<commit_message>
Added 2018 NFL Conference Championship Forecasts
</commit_message>
<xml_diff>
--- a/NFL2018/Weekly Forecasts/WeekDivMatrix.xlsx
+++ b/NFL2018/Weekly Forecasts/WeekDivMatrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2018\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9ECE936F-5A40-45D2-9CA9-3E73A7D02D62}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0FFD2EE3-0BE2-4180-8004-E3C40256EDBF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projected Bracket" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="49">
   <si>
     <t>Chance of Winning</t>
   </si>
@@ -193,12 +193,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0%"/>
     <numFmt numFmtId="165" formatCode="#0.0"/>
     <numFmt numFmtId="166" formatCode="#0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +273,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -653,10 +661,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -721,10 +730,10 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -733,13 +742,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -811,37 +820,39 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="16" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="16" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1179,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDB5B8D-F814-4F70-AC5B-07B019C4E841}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -1593,10 +1604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858EF976-FCF4-4411-B313-E6B56EE0E7AC}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2155,6 +2166,14 @@
         <f>E2</f>
         <v>0.58312478337504337</v>
       </c>
+      <c r="C12">
+        <f>B12*(B13*C2+B14*D2)</f>
+        <v>0.33425842031468689</v>
+      </c>
+      <c r="D12">
+        <f>C12*MMULT(F2:I2, $C$16:$C$19)</f>
+        <v>0.18233013841206774</v>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
@@ -2165,6 +2184,14 @@
         <f>D3</f>
         <v>0.55317458936508213</v>
       </c>
+      <c r="C13">
+        <f>B13*(B12*B3+B15*E3)</f>
+        <v>0.26815894739469209</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D15" si="6">C13*MMULT(F3:I3, $C$16:$C$19)</f>
+        <v>0.13334457383156384</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
@@ -2175,6 +2202,14 @@
         <f>C4</f>
         <v>0.44682541063491787</v>
       </c>
+      <c r="C14">
+        <f>B14*(B12*B4+B15*E4)</f>
+        <v>0.19967294661695686</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="6"/>
+        <v>9.4785269334924135E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="str">
@@ -2185,6 +2220,14 @@
         <f>B5</f>
         <v>0.41687521662495663</v>
       </c>
+      <c r="C15">
+        <f>B15*(B13*C5+B14*D5)</f>
+        <v>0.19790968567366415</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="6"/>
+        <v>9.257843961625338E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="str">
@@ -2195,8 +2238,16 @@
         <f>I6</f>
         <v>0.6704424659115068</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <f>B16*(B17*G6+B18*H6)</f>
+        <v>0.38865384403902697</v>
+      </c>
+      <c r="D16">
+        <f>C16*MMULT(B6:E6, $C$12:$C$15)</f>
+        <v>0.21493622961254838</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
         <f t="shared" si="5"/>
         <v>LAR</v>
@@ -2205,8 +2256,16 @@
         <f>H7</f>
         <v>0.65787906842418631</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <f>B17*(B16*F7+B19*I7)</f>
+        <v>0.34761800736512127</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:D19" si="7">C17*MMULT(B7:E7, $C$12:$C$15)</f>
+        <v>0.18283501219089665</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="5"/>
         <v>DAL</v>
@@ -2215,8 +2274,16 @@
         <f>G8</f>
         <v>0.34212093157581369</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <f>B18*(B16*F8+B19*I8)</f>
+        <v>0.13120022739267034</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>4.935168072596597E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="5"/>
         <v>PHI</v>
@@ -2225,8 +2292,99 @@
         <f>F9</f>
         <v>0.3295575340884932</v>
       </c>
+      <c r="C19">
+        <f>B19*(B17*G9+B18*H9)</f>
+        <v>0.13252792120318138</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="7"/>
+        <v>4.9838656275779901E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="62">
+        <f>VLOOKUP(A22, $A$12:$D$19, 4, FALSE)</f>
+        <v>0.21493622961254838</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="62">
+        <f>VLOOKUP(A23, $A$12:$D$19, 4, FALSE)</f>
+        <v>0.18283501219089665</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="62">
+        <f>VLOOKUP(A24, $A$12:$D$19, 4, FALSE)</f>
+        <v>0.18233013841206774</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="62">
+        <f>VLOOKUP(A25, $A$12:$D$19, 4, FALSE)</f>
+        <v>0.13334457383156384</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="62">
+        <f>VLOOKUP(A26, $A$12:$D$19, 4, FALSE)</f>
+        <v>9.4785269334924135E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="62">
+        <f>VLOOKUP(A27, $A$12:$D$19, 4, FALSE)</f>
+        <v>9.257843961625338E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="62">
+        <f>VLOOKUP(A28, $A$12:$D$19, 4, FALSE)</f>
+        <v>4.9838656275779901E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="62">
+        <f>VLOOKUP(A29, $A$12:$D$19, 4, FALSE)</f>
+        <v>4.935168072596597E-2</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A22:B29">
+    <sortCondition descending="1" ref="B22"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>